<commit_message>
add mine's project proposals
</commit_message>
<xml_diff>
--- a/Projects/Project 1/Mine_Sta 101 S15 - Project Proposal.xlsx
+++ b/Projects/Project 1/Mine_Sta 101 S15 - Project Proposal.xlsx
@@ -1,12 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <workbookPr autoCompressPictures="0"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="1080" windowWidth="25600" windowHeight="14980" tabRatio="500"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Proposals" state="visible" r:id="rId3"/>
+    <sheet name="Proposals" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -136,8 +144,7 @@
     <t>Is there a relationship between level of education completed and frequency of smoking cigarettes?</t>
   </si>
   <si>
-    <t>There are 491,773 cases of non-institutionalized adults, aged 18 years or older, who reside in the US that are considered in this population. 
-</t>
+    <t>There are 491,773 cases of non-institutionalized adults, aged 18 years or older, who reside in the US that are considered in this population.</t>
   </si>
   <si>
     <t>Since 2011, BRFSS conducts both landline telephone- and cellular telephone-based surveys. In conducting the BRFSS landline telephone survey, interviewers collect data from a randomly selected adult in a household. In conducting the cellular telephone version of the BRFSS questionnaire, interviewers collect data from an adult who participates by using a cellular telephone and resides in a private residence or college housing. This is random sampling in that the landline telephone- and cellular users were randomly selected, as were the individuals  in the household. However, there is convenience bias since they are  only surveying those with access to telephone services. There also may be non-response bias as there is no enforced requirement to participate in the survey, there may be people were contacted who declined to participate in the survey.</t>
@@ -194,8 +201,7 @@
     <t xml:space="preserve">There are 1540 cases total. Each case is a person who took the General Social Survey (GSS)  in 2002 and provided information about both health and doctor. </t>
   </si>
   <si>
-    <t>The General Social Survey (GSS) is a sociological survey used to collect data on demographic characteristics and attitudes of residents of the United States. The survey is conducted face-to-face with an in-person interview by the National Opinion Research Center at the University of Chicago, of adults (18+) in randomly selected households. 
-</t>
+    <t>The General Social Survey (GSS) is a sociological survey used to collect data on demographic characteristics and attitudes of residents of the United States. The survey is conducted face-to-face with an in-person interview by the National Opinion Research Center at the University of Chicago, of adults (18+) in randomly selected households.</t>
   </si>
   <si>
     <t>This is an observational study.</t>
@@ -204,12 +210,10 @@
     <t>https://docs.google.com/spreadsheets/d/1hgH3fDWDTpW2jN_pgvb3rjboiXcs8N1poqTrA4GQocY/edit?usp=sharing</t>
   </si>
   <si>
-    <t>Our response variable is health (self-reported) and is a categorical variable with 4 levels.
-</t>
-  </si>
-  <si>
-    <t>Our explanatory variable is the doctor (whether or not the patient reports having a regular doctor) and is also a categorical variable, but with only 2 levels.
-</t>
+    <t>Our response variable is health (self-reported) and is a categorical variable with 4 levels.</t>
+  </si>
+  <si>
+    <t>Our explanatory variable is the doctor (whether or not the patient reports having a regular doctor) and is also a categorical variable, but with only 2 levels.</t>
   </si>
   <si>
     <t xml:space="preserve">Since both of our variables are categorical, it would not make sense to calculate means and SDs, but we were able to find the proportions of  self-reported health by respondents within both groups, those with and those without doctors. </t>
@@ -382,8 +386,7 @@
   </si>
   <si>
     <t>The cohort contains responses from 491,773 people. Each case is one person’s response. For the questions of interest (avdrnk2 &amp; educa),  the response rate varied.
-We’re considering “missing” data responses to be equivalent to “refused to answer” because the differential attrition and response rates for the two variables complicate the data analysis beyond the scope of our course. As such, there are 491,773 cases for both variables even with non-responses and missing answers.
-</t>
+We’re considering “missing” data responses to be equivalent to “refused to answer” because the differential attrition and response rates for the two variables complicate the data analysis beyond the scope of our course. As such, there are 491,773 cases for both variables even with non-responses and missing answers.</t>
   </si>
   <si>
     <t>We’re going to use a retrospective cohort from the Behavioral Risk Factor Surveillance System. The study was a telephone study conducted in all 50 states, the District of Columbia, Puerto Rico, Guam, and the US Virgin Islands. Respondents were over 18 years of age.</t>
@@ -438,8 +441,7 @@
     <t>Is there a relationship between age and view on premarital sex?</t>
   </si>
   <si>
-    <t>The cases are 16127 respondents. We are looking at responses collected from 2000-2012
-</t>
+    <t>The cases are 16127 respondents. We are looking at responses collected from 2000-2012</t>
   </si>
   <si>
     <t>Data is collected through face-face in-person interviews with adults aged 18 and older in randomly selected households</t>
@@ -477,8 +479,7 @@
     <t>http://guides.library.duke.edu/content.php?pid=380130&amp;sid=3136477</t>
   </si>
   <si>
-    <t>The response variable is the survey participant’s answer of “Yes/No” to the question. It is categorical.
-</t>
+    <t>The response variable is the survey participant’s answer of “Yes/No” to the question. It is categorical.</t>
   </si>
   <si>
     <t>The explanatory variable is the year. It is categorical.</t>
@@ -630,8 +631,7 @@
     <t>How often have you felt depressed in the last 30 days --&gt; categorical (ordinal)</t>
   </si>
   <si>
-    <t>Hours of sleep per night --&gt; numerical (discrete)
-</t>
+    <t>Hours of sleep per night --&gt; numerical (discrete)</t>
   </si>
   <si>
     <t>Stat-tastic 4</t>
@@ -843,35 +843,47 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
-    </font>
-    <font/>
-    <font>
-      <u/>
-      <color rgb="FF0000FF"/>
+      <sz val="12"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -879,7 +891,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -907,1145 +919,1460 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1" applyFill="1">
-      <alignment/>
-    </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
-      <alignment/>
-    </xf>
-    <xf applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3" applyFill="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="4">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="5">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="6">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3">
-      <alignment/>
-    </xf>
-    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="7">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane topLeftCell="B3" ySplit="2.0" xSplit="1.0" activePane="bottomRight" state="frozen"/>
-      <selection sqref="B1" activeCell="B1" pane="topRight"/>
-      <selection sqref="A3" activeCell="A3" pane="bottomLeft"/>
-      <selection sqref="B3" activeCell="B3" pane="bottomRight"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="I22" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" customWidth="1" max="3" width="37.71"/>
-    <col min="4" customWidth="1" max="4" width="74.29"/>
-    <col min="5" customWidth="1" max="5" width="25.0"/>
-    <col min="6" customWidth="1" max="6" width="29.71"/>
-    <col min="7" customWidth="1" max="7" width="59.14"/>
-    <col min="8" customWidth="1" max="8" width="69.71"/>
-    <col min="9" customWidth="1" max="9" width="72.57"/>
-    <col min="10" customWidth="1" max="10" width="61.71"/>
-    <col min="11" customWidth="1" max="11" width="97.43"/>
+    <col min="1" max="3" width="37.6640625" customWidth="1"/>
+    <col min="4" max="4" width="74.33203125" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="29.6640625" customWidth="1"/>
+    <col min="7" max="7" width="59.1640625" customWidth="1"/>
+    <col min="8" max="8" width="69.6640625" customWidth="1"/>
+    <col min="9" max="9" width="72.5" customWidth="1"/>
+    <col min="10" max="10" width="61.6640625" customWidth="1"/>
+    <col min="11" max="11" width="97.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c s="1" r="A1"/>
-      <c t="s" s="1" r="B1">
+    <row r="1" spans="1:11" ht="36">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="1" r="C1">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c t="s" s="1" r="D1">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="1" r="E1">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c t="s" s="1" r="F1">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c t="s" s="1" r="G1">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c t="s" s="1" r="H1">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c t="s" s="1" r="I1">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="1" r="J1">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c t="s" s="2" r="K1">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row customHeight="1" r="2" ht="12.0">
-      <c t="s" s="3" r="A2">
+    <row r="2" spans="1:11" ht="12" customHeight="1">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c t="s" s="3" r="B2">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="3" r="C2">
+      <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="3" r="D2">
+      <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c t="s" s="3" r="E2">
+      <c r="E2" s="3" t="s">
         <v>14</v>
       </c>
-      <c t="s" s="3" r="F2">
+      <c r="F2" s="3" t="s">
         <v>15</v>
       </c>
-      <c t="s" s="3" r="G2">
+      <c r="G2" s="3" t="s">
         <v>16</v>
       </c>
-      <c t="s" s="3" r="H2">
+      <c r="H2" s="3" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="3" r="I2">
+      <c r="I2" s="3" t="s">
         <v>18</v>
       </c>
-      <c t="s" s="3" r="J2">
+      <c r="J2" s="3" t="s">
         <v>19</v>
       </c>
-      <c t="s" s="4" r="K2">
+      <c r="K2" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row customHeight="1" r="3" ht="88.5">
-      <c t="s" s="5" r="A3">
+    <row r="3" spans="1:11" ht="88.5" customHeight="1">
+      <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
-      <c t="s" s="5" r="B3">
+      <c r="B3" s="5" t="s">
         <v>22</v>
       </c>
-      <c t="s" s="5" r="C3">
+      <c r="C3" s="5" t="s">
         <v>23</v>
       </c>
-      <c t="s" s="5" r="D3">
+      <c r="D3" s="5" t="s">
         <v>24</v>
       </c>
-      <c t="s" s="5" r="E3">
+      <c r="E3" s="5" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="5" r="F3">
+      <c r="F3" s="5" t="s">
         <v>26</v>
       </c>
-      <c t="s" s="6" r="G3">
+      <c r="G3" s="6" t="s">
         <v>27</v>
       </c>
-      <c t="s" s="5" r="H3">
+      <c r="H3" s="5" t="s">
         <v>28</v>
       </c>
-      <c t="s" s="5" r="I3">
+      <c r="I3" s="5" t="s">
         <v>29</v>
       </c>
-      <c t="s" s="5" r="J3">
+      <c r="J3" s="5" t="s">
         <v>30</v>
       </c>
-      <c s="7" r="K3"/>
-    </row>
-    <row customHeight="1" r="4" ht="39.0">
-      <c t="s" s="8" r="A4">
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" ht="39" customHeight="1">
+      <c r="A4" s="8" t="s">
         <v>31</v>
       </c>
-      <c t="s" s="8" r="B4">
+      <c r="B4" s="8" t="s">
         <v>32</v>
       </c>
-      <c t="s" s="8" r="C4">
+      <c r="C4" s="8" t="s">
         <v>33</v>
       </c>
-      <c t="s" s="8" r="D4">
+      <c r="D4" s="8" t="s">
         <v>34</v>
       </c>
-      <c t="s" s="8" r="E4">
+      <c r="E4" s="8" t="s">
         <v>35</v>
       </c>
-      <c s="8" r="F4"/>
-      <c s="8" r="G4"/>
-      <c t="s" s="8" r="H4">
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="8" r="I4">
+      <c r="I4" s="8" t="s">
         <v>37</v>
       </c>
-      <c t="s" s="8" r="J4">
+      <c r="J4" s="8" t="s">
         <v>38</v>
       </c>
-      <c s="7" r="K4"/>
-    </row>
-    <row customHeight="1" r="5" ht="39.0">
-      <c t="s" s="5" r="A5">
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" ht="39" customHeight="1">
+      <c r="A5" s="5" t="s">
         <v>39</v>
       </c>
-      <c t="s" s="5" r="B5">
+      <c r="B5" s="5" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="5" r="C5">
+      <c r="C5" s="5" t="s">
         <v>41</v>
       </c>
-      <c t="s" s="5" r="D5">
+      <c r="D5" s="5" t="s">
         <v>42</v>
       </c>
-      <c t="s" s="5" r="E5">
+      <c r="E5" s="5" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="5" r="F5">
+      <c r="F5" s="5" t="s">
         <v>43</v>
       </c>
-      <c t="s" s="6" r="G5">
+      <c r="G5" s="6" t="s">
         <v>44</v>
       </c>
-      <c t="s" s="5" r="H5">
+      <c r="H5" s="5" t="s">
         <v>45</v>
       </c>
-      <c t="s" s="5" r="I5">
+      <c r="I5" s="5" t="s">
         <v>46</v>
       </c>
-      <c t="s" s="5" r="J5">
+      <c r="J5" s="5" t="s">
         <v>47</v>
       </c>
-      <c s="7" r="K5"/>
-    </row>
-    <row customHeight="1" r="6" ht="39.0">
-      <c t="s" s="9" r="A6">
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:11" ht="39" customHeight="1">
+      <c r="A6" s="9" t="s">
         <v>48</v>
       </c>
-      <c t="s" s="9" r="B6">
+      <c r="B6" s="9" t="s">
         <v>49</v>
       </c>
-      <c t="s" s="9" r="C6">
+      <c r="C6" s="9" t="s">
         <v>50</v>
       </c>
-      <c t="s" s="9" r="D6">
+      <c r="D6" s="9" t="s">
         <v>51</v>
       </c>
-      <c t="s" s="9" r="E6">
+      <c r="E6" s="9" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="9" r="F6">
+      <c r="F6" s="9" t="s">
         <v>52</v>
       </c>
-      <c t="s" s="9" r="G6">
+      <c r="G6" s="9" t="s">
         <v>53</v>
       </c>
-      <c t="s" s="9" r="H6">
+      <c r="H6" s="9" t="s">
         <v>54</v>
       </c>
-      <c t="s" s="9" r="I6">
+      <c r="I6" s="9" t="s">
         <v>55</v>
       </c>
-      <c t="s" s="9" r="J6">
+      <c r="J6" s="9" t="s">
         <v>56</v>
       </c>
-      <c s="7" r="K6"/>
-    </row>
-    <row customHeight="1" r="7" ht="39.0">
-      <c t="s" s="5" r="A7">
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="1:11" ht="39" customHeight="1">
+      <c r="A7" s="5" t="s">
         <v>57</v>
       </c>
-      <c t="s" s="5" r="B7">
+      <c r="B7" s="5" t="s">
         <v>58</v>
       </c>
-      <c t="s" s="5" r="C7">
+      <c r="C7" s="5" t="s">
         <v>59</v>
       </c>
-      <c t="s" s="5" r="D7">
+      <c r="D7" s="5" t="s">
         <v>60</v>
       </c>
-      <c t="s" s="5" r="E7">
+      <c r="E7" s="5" t="s">
         <v>61</v>
       </c>
-      <c t="s" s="5" r="F7">
+      <c r="F7" s="5" t="s">
         <v>52</v>
       </c>
-      <c t="s" s="6" r="G7">
+      <c r="G7" s="6" t="s">
         <v>62</v>
       </c>
-      <c t="s" s="5" r="H7">
+      <c r="H7" s="5" t="s">
         <v>63</v>
       </c>
-      <c t="s" s="5" r="I7">
+      <c r="I7" s="5" t="s">
         <v>64</v>
       </c>
-      <c t="s" s="5" r="J7">
+      <c r="J7" s="5" t="s">
         <v>65</v>
       </c>
-      <c s="7" r="K7"/>
-    </row>
-    <row customHeight="1" r="8" ht="39.0">
-      <c t="s" s="8" r="A8">
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" ht="39" customHeight="1">
+      <c r="A8" s="8" t="s">
         <v>66</v>
       </c>
-      <c t="s" s="8" r="B8">
+      <c r="B8" s="8" t="s">
         <v>67</v>
       </c>
-      <c t="s" s="8" r="C8">
+      <c r="C8" s="8" t="s">
         <v>68</v>
       </c>
-      <c t="s" s="8" r="D8">
+      <c r="D8" s="8" t="s">
         <v>69</v>
       </c>
-      <c t="s" s="8" r="E8">
+      <c r="E8" s="8" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="8" r="F8">
+      <c r="F8" s="8" t="s">
         <v>70</v>
       </c>
-      <c s="8" r="G8"/>
-      <c t="s" s="8" r="H8">
+      <c r="G8" s="8"/>
+      <c r="H8" s="8" t="s">
         <v>71</v>
       </c>
-      <c t="s" s="8" r="I8">
+      <c r="I8" s="8" t="s">
         <v>72</v>
       </c>
-      <c t="s" s="8" r="J8">
+      <c r="J8" s="8" t="s">
         <v>73</v>
       </c>
-      <c s="7" r="K8"/>
-    </row>
-    <row customHeight="1" r="9" ht="39.0">
-      <c t="s" s="5" r="A9">
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" ht="39" customHeight="1">
+      <c r="A9" s="5" t="s">
         <v>74</v>
       </c>
-      <c t="s" s="5" r="B9">
+      <c r="B9" s="5" t="s">
         <v>75</v>
       </c>
-      <c t="s" s="5" r="C9">
+      <c r="C9" s="5" t="s">
         <v>76</v>
       </c>
-      <c t="s" s="5" r="D9">
+      <c r="D9" s="5" t="s">
         <v>77</v>
       </c>
-      <c t="s" s="5" r="E9">
+      <c r="E9" s="5" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="5" r="F9">
+      <c r="F9" s="5" t="s">
         <v>78</v>
       </c>
-      <c s="5" r="G9"/>
-      <c t="s" s="5" r="H9">
+      <c r="G9" s="5"/>
+      <c r="H9" s="5" t="s">
         <v>79</v>
       </c>
-      <c t="s" s="5" r="I9">
+      <c r="I9" s="5" t="s">
         <v>80</v>
       </c>
-      <c t="s" s="5" r="J9">
+      <c r="J9" s="5" t="s">
         <v>81</v>
       </c>
-      <c s="7" r="K9"/>
-    </row>
-    <row customHeight="1" r="10" ht="39.0">
-      <c t="s" s="8" r="A10">
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" ht="39" customHeight="1">
+      <c r="A10" s="8" t="s">
         <v>82</v>
       </c>
-      <c t="s" s="8" r="B10">
+      <c r="B10" s="8" t="s">
         <v>83</v>
       </c>
-      <c t="s" s="8" r="C10">
+      <c r="C10" s="8" t="s">
         <v>84</v>
       </c>
-      <c t="s" s="8" r="D10">
+      <c r="D10" s="8" t="s">
         <v>85</v>
       </c>
-      <c t="s" s="8" r="E10">
+      <c r="E10" s="8" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="8" r="F10">
+      <c r="F10" s="8" t="s">
         <v>52</v>
       </c>
-      <c s="8" r="G10"/>
-      <c t="s" s="8" r="H10">
+      <c r="G10" s="8"/>
+      <c r="H10" s="8" t="s">
         <v>86</v>
       </c>
-      <c t="s" s="8" r="I10">
+      <c r="I10" s="8" t="s">
         <v>87</v>
       </c>
-      <c t="s" s="8" r="J10">
+      <c r="J10" s="8" t="s">
         <v>88</v>
       </c>
-      <c s="7" r="K10"/>
-    </row>
-    <row customHeight="1" r="11" ht="39.0">
-      <c t="s" s="5" r="A11">
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:11" ht="39" customHeight="1">
+      <c r="A11" s="5" t="s">
         <v>89</v>
       </c>
-      <c t="s" s="5" r="B11">
+      <c r="B11" s="5" t="s">
         <v>90</v>
       </c>
-      <c t="s" s="5" r="C11">
+      <c r="C11" s="5" t="s">
         <v>91</v>
       </c>
-      <c t="s" s="5" r="D11">
+      <c r="D11" s="5" t="s">
         <v>92</v>
       </c>
-      <c t="s" s="5" r="E11">
+      <c r="E11" s="5" t="s">
         <v>93</v>
       </c>
-      <c t="s" s="5" r="F11">
+      <c r="F11" s="5" t="s">
         <v>52</v>
       </c>
-      <c s="5" r="G11"/>
-      <c t="s" s="5" r="H11">
+      <c r="G11" s="5"/>
+      <c r="H11" s="5" t="s">
         <v>94</v>
       </c>
-      <c t="s" s="5" r="I11">
+      <c r="I11" s="5" t="s">
         <v>95</v>
       </c>
-      <c t="s" s="5" r="J11">
+      <c r="J11" s="5" t="s">
         <v>96</v>
       </c>
-      <c s="7" r="K11"/>
-    </row>
-    <row customHeight="1" r="12" ht="39.0">
-      <c t="s" s="8" r="A12">
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:11" ht="39" customHeight="1">
+      <c r="A12" s="8" t="s">
         <v>97</v>
       </c>
-      <c t="s" s="8" r="B12">
+      <c r="B12" s="8" t="s">
         <v>98</v>
       </c>
-      <c t="s" s="8" r="C12">
+      <c r="C12" s="8" t="s">
         <v>99</v>
       </c>
-      <c t="s" s="8" r="D12">
+      <c r="D12" s="8" t="s">
         <v>100</v>
       </c>
-      <c t="s" s="8" r="E12">
+      <c r="E12" s="8" t="s">
         <v>101</v>
       </c>
-      <c t="s" s="8" r="F12">
+      <c r="F12" s="8" t="s">
         <v>70</v>
       </c>
-      <c t="s" s="10" r="G12">
+      <c r="G12" s="10" t="s">
         <v>102</v>
       </c>
-      <c t="s" s="8" r="H12">
+      <c r="H12" s="8" t="s">
         <v>103</v>
       </c>
-      <c t="s" s="8" r="I12">
+      <c r="I12" s="8" t="s">
         <v>104</v>
       </c>
-      <c t="s" s="8" r="J12">
+      <c r="J12" s="8" t="s">
         <v>105</v>
       </c>
-      <c s="11" r="K12"/>
-    </row>
-    <row customHeight="1" r="13" ht="39.0">
-      <c t="s" s="5" r="A13">
+      <c r="K12" s="11"/>
+    </row>
+    <row r="13" spans="1:11" ht="39" customHeight="1">
+      <c r="A13" s="5" t="s">
         <v>106</v>
       </c>
-      <c t="s" s="5" r="B13">
+      <c r="B13" s="5" t="s">
         <v>107</v>
       </c>
-      <c t="s" s="5" r="C13">
+      <c r="C13" s="5" t="s">
         <v>108</v>
       </c>
-      <c t="s" s="5" r="D13">
+      <c r="D13" s="5" t="s">
         <v>109</v>
       </c>
-      <c t="s" s="5" r="E13">
+      <c r="E13" s="5" t="s">
         <v>93</v>
       </c>
-      <c t="s" s="5" r="F13">
+      <c r="F13" s="5" t="s">
         <v>110</v>
       </c>
-      <c s="5" r="G13"/>
-      <c t="s" s="5" r="H13">
+      <c r="G13" s="5"/>
+      <c r="H13" s="5" t="s">
         <v>111</v>
       </c>
-      <c t="s" s="5" r="I13">
+      <c r="I13" s="5" t="s">
         <v>112</v>
       </c>
-      <c s="5" r="J13"/>
-      <c s="7" r="K13"/>
-    </row>
-    <row customHeight="1" r="14" ht="39.0">
-      <c t="s" s="8" r="A14">
+      <c r="J13" s="5"/>
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="1:11" ht="39" customHeight="1">
+      <c r="A14" s="8" t="s">
         <v>113</v>
       </c>
-      <c t="s" s="8" r="B14">
+      <c r="B14" s="8" t="s">
         <v>114</v>
       </c>
-      <c t="s" s="8" r="C14">
+      <c r="C14" s="8" t="s">
         <v>115</v>
       </c>
-      <c t="s" s="8" r="D14">
+      <c r="D14" s="8" t="s">
         <v>116</v>
       </c>
-      <c t="s" s="8" r="E14">
+      <c r="E14" s="8" t="s">
         <v>93</v>
       </c>
-      <c t="s" s="8" r="F14">
+      <c r="F14" s="8" t="s">
         <v>110</v>
       </c>
-      <c s="8" r="G14"/>
-      <c t="s" s="8" r="H14">
+      <c r="G14" s="8"/>
+      <c r="H14" s="8" t="s">
         <v>117</v>
       </c>
-      <c t="s" s="8" r="I14">
+      <c r="I14" s="8" t="s">
         <v>118</v>
       </c>
-      <c s="8" r="J14"/>
-      <c s="7" r="K14"/>
-    </row>
-    <row customHeight="1" r="15" ht="39.0">
-      <c t="s" s="5" r="A15">
+      <c r="J14" s="8"/>
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="1:11" ht="39" customHeight="1">
+      <c r="A15" s="5" t="s">
         <v>119</v>
       </c>
-      <c t="s" s="5" r="B15">
+      <c r="B15" s="5" t="s">
         <v>120</v>
       </c>
-      <c t="s" s="5" r="C15">
+      <c r="C15" s="5" t="s">
         <v>121</v>
       </c>
-      <c t="s" s="5" r="D15">
+      <c r="D15" s="5" t="s">
         <v>122</v>
       </c>
-      <c t="s" s="5" r="E15">
+      <c r="E15" s="5" t="s">
         <v>123</v>
       </c>
-      <c t="s" s="6" r="F15">
+      <c r="F15" s="6" t="s">
         <v>124</v>
       </c>
-      <c s="5" r="G15"/>
-      <c t="s" s="5" r="H15">
+      <c r="G15" s="5"/>
+      <c r="H15" s="5" t="s">
         <v>125</v>
       </c>
-      <c t="s" s="5" r="I15">
+      <c r="I15" s="5" t="s">
         <v>126</v>
       </c>
-      <c t="s" s="5" r="J15">
+      <c r="J15" s="5" t="s">
         <v>127</v>
       </c>
-      <c s="11" r="K15"/>
-    </row>
-    <row customHeight="1" r="16" ht="39.0">
-      <c t="s" s="8" r="A16">
+      <c r="K15" s="11"/>
+    </row>
+    <row r="16" spans="1:11" ht="39" customHeight="1">
+      <c r="A16" s="8" t="s">
         <v>128</v>
       </c>
-      <c t="s" s="8" r="B16">
+      <c r="B16" s="8" t="s">
         <v>129</v>
       </c>
-      <c t="s" s="8" r="C16">
+      <c r="C16" s="8" t="s">
         <v>130</v>
       </c>
-      <c t="s" s="8" r="D16">
+      <c r="D16" s="8" t="s">
         <v>131</v>
       </c>
-      <c t="s" s="8" r="E16">
+      <c r="E16" s="8" t="s">
         <v>61</v>
       </c>
-      <c t="s" s="8" r="F16">
+      <c r="F16" s="8" t="s">
         <v>132</v>
       </c>
-      <c t="s" s="10" r="G16">
+      <c r="G16" s="10" t="s">
         <v>133</v>
       </c>
-      <c t="s" s="8" r="H16">
+      <c r="H16" s="8" t="s">
         <v>134</v>
       </c>
-      <c t="s" s="8" r="I16">
+      <c r="I16" s="8" t="s">
         <v>135</v>
       </c>
-      <c t="s" s="8" r="J16">
+      <c r="J16" s="8" t="s">
         <v>136</v>
       </c>
-      <c s="7" r="K16"/>
-    </row>
-    <row customHeight="1" r="17" ht="39.0">
-      <c t="s" s="5" r="A17">
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="1:11" ht="39" customHeight="1">
+      <c r="A17" s="5" t="s">
         <v>137</v>
       </c>
-      <c t="s" s="5" r="B17">
+      <c r="B17" s="5" t="s">
         <v>138</v>
       </c>
-      <c t="s" s="5" r="C17">
+      <c r="C17" s="5" t="s">
         <v>139</v>
       </c>
-      <c t="s" s="5" r="D17">
+      <c r="D17" s="5" t="s">
         <v>140</v>
       </c>
-      <c t="s" s="5" r="E17">
+      <c r="E17" s="5" t="s">
         <v>141</v>
       </c>
-      <c t="s" s="5" r="F17">
+      <c r="F17" s="5" t="s">
         <v>52</v>
       </c>
-      <c t="s" s="6" r="G17">
+      <c r="G17" s="6" t="s">
         <v>142</v>
       </c>
-      <c t="s" s="5" r="H17">
+      <c r="H17" s="5" t="s">
         <v>143</v>
       </c>
-      <c t="s" s="5" r="I17">
+      <c r="I17" s="5" t="s">
         <v>144</v>
       </c>
-      <c s="5" r="J17"/>
-      <c s="7" r="K17"/>
-    </row>
-    <row customHeight="1" r="18" ht="39.0">
-      <c t="s" s="8" r="A18">
+      <c r="J17" s="5"/>
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="1:11" ht="39" customHeight="1">
+      <c r="A18" s="8" t="s">
         <v>145</v>
       </c>
-      <c t="s" s="8" r="B18">
+      <c r="B18" s="8" t="s">
         <v>146</v>
       </c>
-      <c t="s" s="8" r="C18">
+      <c r="C18" s="8" t="s">
         <v>147</v>
       </c>
-      <c t="s" s="8" r="D18">
+      <c r="D18" s="8" t="s">
         <v>148</v>
       </c>
-      <c t="s" s="8" r="E18">
+      <c r="E18" s="8" t="s">
         <v>149</v>
       </c>
-      <c t="s" s="10" r="F18">
+      <c r="F18" s="10" t="s">
         <v>150</v>
       </c>
-      <c s="8" r="G18"/>
-      <c t="s" s="8" r="H18">
+      <c r="G18" s="8"/>
+      <c r="H18" s="8" t="s">
         <v>151</v>
       </c>
-      <c t="s" s="8" r="I18">
+      <c r="I18" s="8" t="s">
         <v>152</v>
       </c>
-      <c t="s" s="8" r="J18">
+      <c r="J18" s="8" t="s">
         <v>153</v>
       </c>
-      <c s="7" r="K18"/>
-    </row>
-    <row customHeight="1" r="19" ht="39.0">
-      <c t="s" s="5" r="A19">
+      <c r="K18" s="7"/>
+    </row>
+    <row r="19" spans="1:11" ht="39" customHeight="1">
+      <c r="A19" s="5" t="s">
         <v>154</v>
       </c>
-      <c t="s" s="5" r="B19">
+      <c r="B19" s="5" t="s">
         <v>155</v>
       </c>
-      <c t="s" s="5" r="C19">
+      <c r="C19" s="5" t="s">
         <v>156</v>
       </c>
-      <c t="s" s="5" r="D19">
+      <c r="D19" s="5" t="s">
         <v>157</v>
       </c>
-      <c t="s" s="5" r="E19">
+      <c r="E19" s="5" t="s">
         <v>123</v>
       </c>
-      <c t="s" s="5" r="F19">
+      <c r="F19" s="5" t="s">
         <v>158</v>
       </c>
-      <c t="s" s="6" r="G19">
+      <c r="G19" s="6" t="s">
         <v>159</v>
       </c>
-      <c t="s" s="5" r="H19">
+      <c r="H19" s="5" t="s">
         <v>160</v>
       </c>
-      <c t="s" s="5" r="I19">
+      <c r="I19" s="5" t="s">
         <v>161</v>
       </c>
-      <c t="s" s="5" r="J19">
+      <c r="J19" s="5" t="s">
         <v>162</v>
       </c>
-      <c s="7" r="K19"/>
-    </row>
-    <row customHeight="1" r="20" ht="39.0">
-      <c t="s" s="8" r="A20">
+      <c r="K19" s="7"/>
+    </row>
+    <row r="20" spans="1:11" ht="39" customHeight="1">
+      <c r="A20" s="8" t="s">
         <v>163</v>
       </c>
-      <c t="s" s="8" r="B20">
+      <c r="B20" s="8" t="s">
         <v>164</v>
       </c>
-      <c t="s" s="8" r="C20">
+      <c r="C20" s="8" t="s">
         <v>165</v>
       </c>
-      <c t="s" s="8" r="D20">
+      <c r="D20" s="8" t="s">
         <v>166</v>
       </c>
-      <c t="s" s="8" r="E20">
+      <c r="E20" s="8" t="s">
         <v>123</v>
       </c>
-      <c t="s" s="8" r="F20">
+      <c r="F20" s="8" t="s">
         <v>167</v>
       </c>
-      <c t="s" s="10" r="G20">
+      <c r="G20" s="10" t="s">
         <v>44</v>
       </c>
-      <c t="s" s="8" r="H20">
+      <c r="H20" s="8" t="s">
         <v>168</v>
       </c>
-      <c t="s" s="8" r="I20">
+      <c r="I20" s="8" t="s">
         <v>169</v>
       </c>
-      <c t="s" s="8" r="J20">
+      <c r="J20" s="8" t="s">
         <v>170</v>
       </c>
-      <c s="12" r="K20"/>
-    </row>
-    <row customHeight="1" r="21" ht="39.0">
-      <c t="s" s="5" r="A21">
+      <c r="K20" s="12"/>
+    </row>
+    <row r="21" spans="1:11" ht="39" customHeight="1">
+      <c r="A21" s="5" t="s">
         <v>171</v>
       </c>
-      <c t="s" s="5" r="B21">
+      <c r="B21" s="5" t="s">
         <v>172</v>
       </c>
-      <c t="s" s="5" r="C21">
+      <c r="C21" s="5" t="s">
         <v>173</v>
       </c>
-      <c t="s" s="5" r="D21">
+      <c r="D21" s="5" t="s">
         <v>174</v>
       </c>
-      <c t="s" s="5" r="E21">
+      <c r="E21" s="5" t="s">
         <v>93</v>
       </c>
-      <c t="s" s="5" r="F21">
+      <c r="F21" s="5" t="s">
         <v>52</v>
       </c>
-      <c t="s" s="5" r="G21">
+      <c r="G21" s="5" t="s">
         <v>175</v>
       </c>
-      <c t="s" s="5" r="H21">
+      <c r="H21" s="5" t="s">
         <v>176</v>
       </c>
-      <c t="s" s="5" r="I21">
+      <c r="I21" s="5" t="s">
         <v>177</v>
       </c>
-      <c t="s" s="5" r="J21">
+      <c r="J21" s="5" t="s">
         <v>178</v>
       </c>
-      <c s="12" r="K21"/>
-    </row>
-    <row customHeight="1" r="22" ht="39.0">
-      <c t="s" s="8" r="A22">
+      <c r="K21" s="12"/>
+    </row>
+    <row r="22" spans="1:11" ht="39" customHeight="1">
+      <c r="A22" s="8" t="s">
         <v>179</v>
       </c>
-      <c t="s" s="8" r="B22">
+      <c r="B22" s="8" t="s">
         <v>180</v>
       </c>
-      <c t="s" s="8" r="C22">
+      <c r="C22" s="8" t="s">
         <v>181</v>
       </c>
-      <c t="s" s="8" r="D22">
+      <c r="D22" s="8" t="s">
         <v>182</v>
       </c>
-      <c t="s" s="8" r="E22">
+      <c r="E22" s="8" t="s">
         <v>93</v>
       </c>
-      <c t="s" s="8" r="F22">
+      <c r="F22" s="8" t="s">
         <v>158</v>
       </c>
-      <c t="s" s="10" r="G22">
+      <c r="G22" s="10" t="s">
         <v>159</v>
       </c>
-      <c t="s" s="8" r="H22">
+      <c r="H22" s="8" t="s">
         <v>183</v>
       </c>
-      <c t="s" s="8" r="I22">
+      <c r="I22" s="8" t="s">
         <v>184</v>
       </c>
-      <c t="s" s="8" r="J22">
+      <c r="J22" s="8" t="s">
         <v>185</v>
       </c>
-      <c s="12" r="K22"/>
-    </row>
-    <row customHeight="1" r="23" ht="39.0">
-      <c t="s" s="5" r="A23">
+      <c r="K22" s="12"/>
+    </row>
+    <row r="23" spans="1:11" ht="39" customHeight="1">
+      <c r="A23" s="5" t="s">
         <v>186</v>
       </c>
-      <c t="s" s="5" r="B23">
+      <c r="B23" s="5" t="s">
         <v>187</v>
       </c>
-      <c t="s" s="5" r="C23">
+      <c r="C23" s="5" t="s">
         <v>188</v>
       </c>
-      <c t="s" s="5" r="D23">
+      <c r="D23" s="5" t="s">
         <v>189</v>
       </c>
-      <c t="s" s="5" r="E23">
+      <c r="E23" s="5" t="s">
         <v>190</v>
       </c>
-      <c t="s" s="5" r="F23">
+      <c r="F23" s="5" t="s">
         <v>52</v>
       </c>
-      <c t="s" s="6" r="G23">
+      <c r="G23" s="6" t="s">
         <v>142</v>
       </c>
-      <c t="s" s="5" r="H23">
+      <c r="H23" s="5" t="s">
         <v>191</v>
       </c>
-      <c t="s" s="5" r="I23">
+      <c r="I23" s="5" t="s">
         <v>161</v>
       </c>
-      <c t="s" s="5" r="J23">
+      <c r="J23" s="5" t="s">
         <v>192</v>
       </c>
-      <c s="7" r="K23"/>
-    </row>
-    <row customHeight="1" r="24" ht="39.0">
-      <c t="s" s="9" r="A24">
+      <c r="K23" s="7"/>
+    </row>
+    <row r="24" spans="1:11" ht="39" customHeight="1">
+      <c r="A24" s="9" t="s">
         <v>193</v>
       </c>
-      <c t="s" s="9" r="B24">
+      <c r="B24" s="9" t="s">
         <v>194</v>
       </c>
-      <c t="s" s="9" r="C24">
+      <c r="C24" s="9" t="s">
         <v>195</v>
       </c>
-      <c t="s" s="9" r="D24">
+      <c r="D24" s="9" t="s">
         <v>196</v>
       </c>
-      <c t="s" s="9" r="E24">
+      <c r="E24" s="9" t="s">
         <v>190</v>
       </c>
-      <c t="s" s="9" r="F24">
+      <c r="F24" s="9" t="s">
         <v>197</v>
       </c>
-      <c t="s" s="13" r="G24">
+      <c r="G24" s="13" t="s">
         <v>198</v>
       </c>
-      <c t="s" s="9" r="H24">
+      <c r="H24" s="9" t="s">
         <v>199</v>
       </c>
-      <c t="s" s="9" r="I24">
+      <c r="I24" s="9" t="s">
         <v>200</v>
       </c>
-      <c s="9" r="J24">
-        <v>13395.0</v>
-      </c>
-      <c s="7" r="K24"/>
-    </row>
-    <row customHeight="1" r="25" ht="39.0">
-      <c t="s" s="5" r="A25">
+      <c r="J24" s="9">
+        <v>13395</v>
+      </c>
+      <c r="K24" s="7"/>
+    </row>
+    <row r="25" spans="1:11" ht="39" customHeight="1">
+      <c r="A25" s="5" t="s">
         <v>201</v>
       </c>
-      <c t="s" s="5" r="B25">
+      <c r="B25" s="5" t="s">
         <v>202</v>
       </c>
-      <c t="s" s="5" r="C25">
+      <c r="C25" s="5" t="s">
         <v>203</v>
       </c>
-      <c t="s" s="5" r="D25">
+      <c r="D25" s="5" t="s">
         <v>204</v>
       </c>
-      <c t="s" s="5" r="E25">
+      <c r="E25" s="5" t="s">
         <v>93</v>
       </c>
-      <c t="s" s="5" r="F25">
+      <c r="F25" s="5" t="s">
         <v>205</v>
       </c>
-      <c t="s" s="6" r="G25">
+      <c r="G25" s="6" t="s">
         <v>198</v>
       </c>
-      <c t="s" s="5" r="H25">
+      <c r="H25" s="5" t="s">
         <v>206</v>
       </c>
-      <c t="s" s="5" r="I25">
+      <c r="I25" s="5" t="s">
         <v>207</v>
       </c>
-      <c t="s" s="5" r="J25">
+      <c r="J25" s="5" t="s">
         <v>208</v>
       </c>
-      <c s="7" r="K25"/>
-    </row>
-    <row customHeight="1" r="26" ht="39.0">
-      <c t="s" s="8" r="A26">
+      <c r="K25" s="7"/>
+    </row>
+    <row r="26" spans="1:11" ht="39" customHeight="1">
+      <c r="A26" s="8" t="s">
         <v>209</v>
       </c>
-      <c t="s" s="8" r="B26">
+      <c r="B26" s="8" t="s">
         <v>210</v>
       </c>
-      <c t="s" s="8" r="C26">
+      <c r="C26" s="8" t="s">
         <v>211</v>
       </c>
-      <c t="s" s="8" r="D26">
+      <c r="D26" s="8" t="s">
         <v>212</v>
       </c>
-      <c t="s" s="8" r="E26">
+      <c r="E26" s="8" t="s">
         <v>213</v>
       </c>
-      <c t="s" s="8" r="F26">
+      <c r="F26" s="8" t="s">
         <v>214</v>
       </c>
-      <c t="s" s="10" r="G26">
+      <c r="G26" s="10" t="s">
         <v>215</v>
       </c>
-      <c t="s" s="8" r="H26">
+      <c r="H26" s="8" t="s">
         <v>216</v>
       </c>
-      <c t="s" s="8" r="I26">
+      <c r="I26" s="8" t="s">
         <v>217</v>
       </c>
-      <c s="8" r="J26">
-        <v>28141.0</v>
-      </c>
-      <c s="7" r="K26"/>
-    </row>
-    <row customHeight="1" r="27" ht="39.0">
-      <c t="s" s="5" r="A27">
+      <c r="J26" s="8">
+        <v>28141</v>
+      </c>
+      <c r="K26" s="7"/>
+    </row>
+    <row r="27" spans="1:11" ht="39" customHeight="1">
+      <c r="A27" s="5" t="s">
         <v>218</v>
       </c>
-      <c t="s" s="5" r="B27">
+      <c r="B27" s="5" t="s">
         <v>219</v>
       </c>
-      <c t="s" s="5" r="C27">
+      <c r="C27" s="5" t="s">
         <v>220</v>
       </c>
-      <c t="s" s="5" r="D27">
+      <c r="D27" s="5" t="s">
         <v>221</v>
       </c>
-      <c t="s" s="5" r="E27">
+      <c r="E27" s="5" t="s">
         <v>222</v>
       </c>
-      <c t="s" s="5" r="F27">
+      <c r="F27" s="5" t="s">
         <v>52</v>
       </c>
-      <c s="5" r="G27"/>
-      <c t="s" s="5" r="H27">
+      <c r="G27" s="5"/>
+      <c r="H27" s="5" t="s">
         <v>223</v>
       </c>
-      <c t="s" s="5" r="I27">
+      <c r="I27" s="5" t="s">
         <v>224</v>
       </c>
-      <c t="s" s="5" r="J27">
+      <c r="J27" s="5" t="s">
         <v>225</v>
       </c>
-      <c s="11" r="K27"/>
-    </row>
-    <row customHeight="1" r="28" ht="39.0">
-      <c t="s" s="8" r="A28">
+      <c r="K27" s="11"/>
+    </row>
+    <row r="28" spans="1:11" ht="39" customHeight="1">
+      <c r="A28" s="8" t="s">
         <v>226</v>
       </c>
-      <c t="s" s="8" r="B28">
+      <c r="B28" s="8" t="s">
         <v>227</v>
       </c>
-      <c t="s" s="8" r="C28">
+      <c r="C28" s="8" t="s">
         <v>228</v>
       </c>
-      <c t="s" s="8" r="D28">
+      <c r="D28" s="8" t="s">
         <v>229</v>
       </c>
-      <c t="s" s="8" r="E28">
+      <c r="E28" s="8" t="s">
         <v>222</v>
       </c>
-      <c t="s" s="8" r="F28">
+      <c r="F28" s="8" t="s">
         <v>230</v>
       </c>
-      <c s="8" r="G28"/>
-      <c t="s" s="8" r="H28">
+      <c r="G28" s="8"/>
+      <c r="H28" s="8" t="s">
         <v>231</v>
       </c>
-      <c t="s" s="8" r="I28">
+      <c r="I28" s="8" t="s">
         <v>232</v>
       </c>
-      <c t="s" s="8" r="J28">
+      <c r="J28" s="8" t="s">
         <v>233</v>
       </c>
-      <c s="7" r="K28"/>
-    </row>
-    <row customHeight="1" r="29" ht="69.75">
-      <c t="s" s="5" r="A29">
+      <c r="K28" s="7"/>
+    </row>
+    <row r="29" spans="1:11" ht="69.75" customHeight="1">
+      <c r="A29" s="5" t="s">
         <v>234</v>
       </c>
-      <c t="s" s="5" r="B29">
+      <c r="B29" s="5" t="s">
         <v>235</v>
       </c>
-      <c t="s" s="5" r="C29">
+      <c r="C29" s="5" t="s">
         <v>236</v>
       </c>
-      <c t="s" s="5" r="D29">
+      <c r="D29" s="5" t="s">
         <v>237</v>
       </c>
-      <c t="s" s="5" r="E29">
+      <c r="E29" s="5" t="s">
         <v>222</v>
       </c>
-      <c t="s" s="5" r="F29">
+      <c r="F29" s="5" t="s">
         <v>238</v>
       </c>
-      <c t="s" s="5" r="G29">
+      <c r="G29" s="5" t="s">
         <v>239</v>
       </c>
-      <c t="s" s="5" r="H29">
+      <c r="H29" s="5" t="s">
         <v>240</v>
       </c>
-      <c t="s" s="5" r="I29">
+      <c r="I29" s="5" t="s">
         <v>241</v>
       </c>
-      <c t="s" s="5" r="J29">
+      <c r="J29" s="14" t="s">
         <v>242</v>
       </c>
-      <c s="11" r="K29"/>
-    </row>
-    <row customHeight="1" r="30" ht="39.0">
-      <c t="s" s="8" r="A30">
+      <c r="K29" s="11"/>
+    </row>
+    <row r="30" spans="1:11" ht="39" customHeight="1">
+      <c r="A30" s="8" t="s">
         <v>243</v>
       </c>
-      <c t="s" s="8" r="B30">
+      <c r="B30" s="8" t="s">
         <v>244</v>
       </c>
-      <c t="s" s="8" r="C30">
+      <c r="C30" s="8" t="s">
         <v>245</v>
       </c>
-      <c t="s" s="8" r="D30">
+      <c r="D30" s="8" t="s">
         <v>246</v>
       </c>
-      <c t="s" s="8" r="E30">
+      <c r="E30" s="8" t="s">
         <v>222</v>
       </c>
-      <c t="s" s="8" r="F30">
+      <c r="F30" s="8" t="s">
         <v>247</v>
       </c>
-      <c t="s" s="10" r="G30">
+      <c r="G30" s="10" t="s">
         <v>248</v>
       </c>
-      <c t="s" s="8" r="H30">
+      <c r="H30" s="8" t="s">
         <v>249</v>
       </c>
-      <c t="s" s="8" r="I30">
+      <c r="I30" s="8" t="s">
         <v>250</v>
       </c>
-      <c s="8" r="J30">
-        <v>134197.0</v>
-      </c>
-      <c s="7" r="K30"/>
-    </row>
-    <row customHeight="1" r="31" ht="69.75">
-      <c t="s" s="5" r="A31">
+      <c r="J30" s="8">
+        <v>134197</v>
+      </c>
+      <c r="K30" s="7"/>
+    </row>
+    <row r="31" spans="1:11" ht="69.75" customHeight="1">
+      <c r="A31" s="5" t="s">
         <v>251</v>
       </c>
-      <c t="s" s="5" r="B31">
+      <c r="B31" s="5" t="s">
         <v>252</v>
       </c>
-      <c t="s" s="5" r="C31">
+      <c r="C31" s="5" t="s">
         <v>253</v>
       </c>
-      <c t="s" s="5" r="D31">
+      <c r="D31" s="5" t="s">
         <v>254</v>
       </c>
-      <c t="s" s="5" r="E31">
+      <c r="E31" s="5" t="s">
         <v>222</v>
       </c>
-      <c t="s" s="5" r="F31">
+      <c r="F31" s="5" t="s">
         <v>255</v>
       </c>
-      <c t="s" s="5" r="G31">
+      <c r="G31" s="5" t="s">
         <v>239</v>
       </c>
-      <c t="s" s="5" r="H31">
+      <c r="H31" s="5" t="s">
         <v>256</v>
       </c>
-      <c t="s" s="5" r="I31">
+      <c r="I31" s="5" t="s">
         <v>257</v>
       </c>
-      <c t="s" s="5" r="J31">
+      <c r="J31" s="5" t="s">
         <v>258</v>
       </c>
-      <c s="12" r="K31"/>
-    </row>
-    <row customHeight="1" r="32" ht="39.0">
-      <c t="s" s="8" r="A32">
+      <c r="K31" s="12"/>
+    </row>
+    <row r="32" spans="1:11" ht="39" customHeight="1">
+      <c r="A32" s="8" t="s">
         <v>259</v>
       </c>
-      <c t="s" s="8" r="B32">
+      <c r="B32" s="8" t="s">
         <v>260</v>
       </c>
-      <c t="s" s="8" r="C32">
+      <c r="C32" s="8" t="s">
         <v>261</v>
       </c>
-      <c t="s" s="8" r="D32">
+      <c r="D32" s="8" t="s">
         <v>262</v>
       </c>
-      <c t="s" s="8" r="E32">
+      <c r="E32" s="8" t="s">
         <v>93</v>
       </c>
-      <c t="s" s="8" r="F32">
+      <c r="F32" s="8" t="s">
         <v>263</v>
       </c>
-      <c t="s" s="8" r="G32">
+      <c r="G32" s="8" t="s">
         <v>239</v>
       </c>
-      <c t="s" s="8" r="H32">
+      <c r="H32" s="8" t="s">
         <v>264</v>
       </c>
-      <c t="s" s="8" r="I32">
+      <c r="I32" s="8" t="s">
         <v>265</v>
       </c>
-      <c t="s" s="8" r="J32">
+      <c r="J32" s="8" t="s">
         <v>266</v>
       </c>
-      <c s="12" r="K32"/>
-    </row>
-    <row customHeight="1" r="33" ht="39.0">
-      <c s="8" r="A33"/>
-      <c s="8" r="B33"/>
-      <c s="8" r="C33"/>
-      <c s="8" r="D33"/>
-      <c s="8" r="E33"/>
-      <c s="8" r="F33"/>
-      <c s="8" r="G33"/>
-      <c s="8" r="H33"/>
-      <c s="8" r="I33"/>
-      <c t="s" s="8" r="J33">
+      <c r="K32" s="12"/>
+    </row>
+    <row r="33" spans="1:11" ht="39" customHeight="1">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8" t="s">
         <v>267</v>
       </c>
-      <c s="12" r="K33"/>
-    </row>
-    <row customHeight="1" r="34" ht="39.0">
-      <c s="8" r="A34"/>
-      <c s="8" r="B34"/>
-      <c s="8" r="C34"/>
-      <c s="8" r="D34"/>
-      <c s="8" r="E34"/>
-      <c s="8" r="F34"/>
-      <c s="8" r="G34"/>
-      <c s="8" r="H34"/>
-      <c s="8" r="I34"/>
-      <c s="8" r="J34">
-        <v>2274.0</v>
-      </c>
-      <c s="12" r="K34"/>
+      <c r="K33" s="12"/>
+    </row>
+    <row r="34" spans="1:11" ht="39" customHeight="1">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8">
+        <v>2274</v>
+      </c>
+      <c r="K34" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2053,7 +2380,7 @@
     <hyperlink ref="G5" r:id="rId2"/>
     <hyperlink ref="G7" r:id="rId3"/>
     <hyperlink ref="G12" r:id="rId4"/>
-    <hyperlink ref="F15" r:id="rId5"/>
+    <hyperlink ref="F15" r:id="rId5" location="#avedrnk2"/>
     <hyperlink ref="G16" r:id="rId6"/>
     <hyperlink ref="G17" r:id="rId7"/>
     <hyperlink ref="F18" r:id="rId8"/>
@@ -2066,6 +2393,11 @@
     <hyperlink ref="G26" r:id="rId15"/>
     <hyperlink ref="G30" r:id="rId16"/>
   </hyperlinks>
-  <drawing r:id="rId17"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>